<commit_message>
Add sub-task 9.3 based on reviewer feedback to Sprint 2 Gantt Chart Planning and Decisions.xlsx
</commit_message>
<xml_diff>
--- a/Project-Management/Sprint 2 Gantt Chart Planning and Decisions.xlsx
+++ b/Project-Management/Sprint 2 Gantt Chart Planning and Decisions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tudublin-my.sharepoint.com/personal/d24126048_mytudublin_ie/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\SafePath\Project-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{5AD82370-A10B-4140-9D7E-28C1BD8D4B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A8D0E63-ABD8-4550-AC30-89EA5A325B20}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C116248-F1B8-4DCE-A2B9-BA5E746D5D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4ABC7AA1-9AD4-4002-AC33-3494CC7CBE2D}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{4ABC7AA1-9AD4-4002-AC33-3494CC7CBE2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart - Dependencies and " sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="72">
   <si>
     <t>Task name</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>Gantt Chart Planning for Sprint 2</t>
+  </si>
+  <si>
+    <t>Conduct competitive analysis and integrate insights into prototype</t>
   </si>
 </sst>
 </file>
@@ -802,10 +805,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1125,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D864422E-3F28-48B7-B5D2-D75C3938ED99}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1865,37 +1864,37 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
+      <c r="A30" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="4">
+        <v>45938</v>
+      </c>
+      <c r="F30" s="4">
+        <v>45941</v>
+      </c>
+      <c r="G30" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>10</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="4">
-        <v>45936</v>
-      </c>
-      <c r="F30" s="4">
-        <v>45938</v>
-      </c>
-      <c r="G30" s="3">
-        <v>1</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A31" s="3">
-        <v>10.1</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>7</v>
@@ -1907,21 +1906,21 @@
         <v>45936</v>
       </c>
       <c r="F31" s="4">
-        <v>45937</v>
+        <v>45938</v>
       </c>
       <c r="G31" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
-        <v>10.199999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>7</v>
@@ -1930,46 +1929,50 @@
         <v>8</v>
       </c>
       <c r="E32" s="4">
+        <v>45936</v>
+      </c>
+      <c r="F32" s="4">
         <v>45937</v>
       </c>
-      <c r="F32" s="4">
+      <c r="G32" s="3">
+        <v>10</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="4">
+        <v>45937</v>
+      </c>
+      <c r="F33" s="4">
         <v>45938</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G33" s="3">
         <v>10.1</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
+    <row r="34" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
         <v>11</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="4">
-        <v>45939</v>
-      </c>
-      <c r="F33" s="4">
-        <v>45940</v>
-      </c>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A34" s="3">
-        <v>11.1</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>38</v>
@@ -1981,21 +1984,17 @@
         <v>45939</v>
       </c>
       <c r="F34" s="4">
-        <v>45939</v>
-      </c>
-      <c r="G34" s="3">
-        <v>11</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>45940</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
-        <v>11.2</v>
+        <v>11.1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>38</v>
@@ -2004,50 +2003,50 @@
         <v>49</v>
       </c>
       <c r="E35" s="4">
-        <v>45940</v>
+        <v>45939</v>
       </c>
       <c r="F35" s="4">
-        <v>45940</v>
+        <v>45939</v>
       </c>
       <c r="G35" s="3">
-        <v>11.1</v>
+        <v>11</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A36" s="2">
-        <v>12</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>53</v>
+      <c r="A36" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="E36" s="4">
         <v>45940</v>
       </c>
       <c r="F36" s="4">
-        <v>45942</v>
+        <v>45940</v>
       </c>
       <c r="G36" s="3">
-        <v>2</v>
+        <v>11.1</v>
       </c>
       <c r="H36" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A37" s="3">
-        <v>12.1</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>54</v>
+      <c r="B37" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>13</v>
@@ -2059,69 +2058,73 @@
         <v>45940</v>
       </c>
       <c r="F37" s="4">
-        <v>45941</v>
+        <v>45942</v>
       </c>
       <c r="G37" s="3">
+        <v>2</v>
+      </c>
+      <c r="H37" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E38" s="4">
+        <v>45940</v>
+      </c>
+      <c r="F38" s="4">
         <v>45941</v>
       </c>
-      <c r="F38" s="4">
+      <c r="G38" s="3">
+        <v>12</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="4">
+        <v>45941</v>
+      </c>
+      <c r="F39" s="4">
         <v>45942</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G39" s="3">
         <v>12.1</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A39" s="2">
+    <row r="40" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
         <v>13</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39" s="4">
-        <v>45936</v>
-      </c>
-      <c r="F39" s="4">
-        <v>45939</v>
-      </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A40" s="3">
-        <v>13.1</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>38</v>
@@ -2133,76 +2136,72 @@
         <v>45936</v>
       </c>
       <c r="F40" s="4">
-        <v>45938</v>
-      </c>
-      <c r="G40" s="3">
-        <v>11</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>45939</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
-        <v>13.2</v>
+        <v>13.1</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E41" s="4">
-        <v>45939</v>
+        <v>45936</v>
       </c>
       <c r="F41" s="4">
-        <v>45939</v>
+        <v>45938</v>
       </c>
       <c r="G41" s="3">
-        <v>13.1</v>
+        <v>11</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A42" s="2">
-        <v>14</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>60</v>
+      <c r="A42" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="E42" s="4">
         <v>45939</v>
       </c>
       <c r="F42" s="4">
-        <v>45943</v>
+        <v>45939</v>
       </c>
       <c r="G42" s="3">
-        <v>6</v>
+        <v>13.1</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A43" s="3">
-        <v>14.1</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>61</v>
+      <c r="A43" s="2">
+        <v>14</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>29</v>
@@ -2211,73 +2210,73 @@
         <v>45939</v>
       </c>
       <c r="F43" s="4">
-        <v>45941</v>
+        <v>45943</v>
       </c>
       <c r="G43" s="3">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
-        <v>14.2</v>
+        <v>14.1</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E44" s="4">
+        <v>45939</v>
+      </c>
+      <c r="F44" s="4">
         <v>45941</v>
       </c>
-      <c r="F44" s="4">
-        <v>45943</v>
-      </c>
       <c r="G44" s="3">
-        <v>14.1</v>
+        <v>14</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A45" s="2">
-        <v>15</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>63</v>
+      <c r="A45" s="3">
+        <v>14.2</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E45" s="4">
-        <v>45936</v>
+        <v>45941</v>
       </c>
       <c r="F45" s="4">
         <v>45943</v>
       </c>
       <c r="G45" s="3">
-        <v>8</v>
+        <v>14.1</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A46" s="3">
-        <v>15.1</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>64</v>
+      <c r="A46" s="2">
+        <v>15</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>17</v>
@@ -2289,10 +2288,10 @@
         <v>45936</v>
       </c>
       <c r="F46" s="4">
-        <v>45942</v>
+        <v>45943</v>
       </c>
       <c r="G46" s="3">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>10</v>
@@ -2300,39 +2299,65 @@
     </row>
     <row r="47" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
-        <v>15.2</v>
+        <v>15.1</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E47" s="4">
+        <v>45936</v>
+      </c>
+      <c r="F47" s="4">
+        <v>45942</v>
+      </c>
+      <c r="G47" s="3">
+        <v>15</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="4">
         <v>45943</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F48" s="4">
         <v>45943</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G48" s="3">
         <v>15.1</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H48" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
+    <row r="49" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>